<commit_message>
[doc] Docs for benchmark
</commit_message>
<xml_diff>
--- a/benchmark general.xlsx
+++ b/benchmark general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ji2\j4\FlowFree-SearchAgents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD399E3-21E9-4352-B2F1-C8855323A65E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F068A985-A979-488A-BF2C-F759860B698E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmark" sheetId="1" r:id="rId1"/>
@@ -1167,13 +1167,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.90625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" customWidth="1"/>
     <col min="4" max="4" width="11.08984375" customWidth="1"/>
     <col min="5" max="5" width="37.36328125" bestFit="1" customWidth="1"/>

</xml_diff>